<commit_message>
fixing test case for transfer with new template
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Sample_transfer_v4_6_0.xlsx
+++ b/backend/fms_core/tests/valid_templates/Sample_transfer_v4_6_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmarcelino/Desktop/freezeman/backend/fms_core/tests/valid_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310ABCE9-B44A-C840-943E-CFDD1B0B7E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC6962C-A46E-764F-BC54-97CB92DEE77E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30040" windowHeight="11580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="27040" windowHeight="11580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleTransfer" sheetId="1" r:id="rId1"/>
@@ -2359,7 +2359,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2526,9 +2526,6 @@
       <c r="D7" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="43" t="s">
-        <v>25</v>
-      </c>
       <c r="F7" s="14" t="s">
         <v>27</v>
       </c>
@@ -2571,9 +2568,8 @@
       <c r="D8" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="43" t="str">
-        <f t="shared" ref="E8:E70" si="0">IF(AND(E$2="Yes",NOT(ISBLANK($C8))),C8,"")</f>
-        <v/>
+      <c r="E8" s="43" t="s">
+        <v>25</v>
       </c>
       <c r="F8" s="14" t="s">
         <v>34</v>
@@ -2645,7 +2641,7 @@
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
       <c r="E10" s="43" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E8:E70" si="0">IF(AND(E$2="Yes",NOT(ISBLANK($C10))),C10,"")</f>
         <v/>
       </c>
       <c r="F10" s="14"/>
@@ -5092,7 +5088,7 @@
       <formula1>"YES,NO"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="E6:E101" xr:uid="{72A3F1FD-443A-694A-8440-492086E68F93}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="E6 E8:E101" xr:uid="{72A3F1FD-443A-694A-8440-492086E68F93}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>